<commit_message>
- improved console and log output so that they are now in sync! Almost ALL console output is now captured in the log   file as well. - fixed logic error when `nexial.outputToCloud` is `true` but Nexial Cloud Integration is not properly set up. - fixed logic to determine chrome log location and file name
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/electron-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/electron-showcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F89C52-0A81-B842-A8B3-952C7F6E15B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B51432-A862-BE44-ABBE-4184FFCD97F9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="440" windowWidth="34120" windowHeight="15740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-380" yWindow="4420" windowWidth="33600" windowHeight="9700" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="451">
   <si>
     <t>description</t>
   </si>
@@ -1406,6 +1406,15 @@
   </si>
   <si>
     <t>//button[@id='button-ipc']</t>
+  </si>
+  <si>
+    <t>//button[@id='button-about' and text()='About']</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>won't work</t>
   </si>
 </sst>
 </file>
@@ -3573,7 +3582,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3808,7 +3817,9 @@
     </row>
     <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>450</v>
+      </c>
       <c r="C9" s="13" t="s">
         <v>53</v>
       </c>
@@ -3839,7 +3850,7 @@
         <v>70</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -3854,7 +3865,9 @@
     </row>
     <row r="11" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>450</v>
+      </c>
       <c r="C11" s="13" t="s">
         <v>53</v>
       </c>
@@ -4265,7 +4278,9 @@
       <c r="B32" s="5"/>
       <c r="C32" s="13"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="E32" s="7" t="s">
+        <v>448</v>
+      </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>

</xml_diff>